<commit_message>
Some db works & Members job contracts
</commit_message>
<xml_diff>
--- a/public/excel/subscribers.xlsx
+++ b/public/excel/subscribers.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
   <si>
     <t>م</t>
   </si>
@@ -32,19 +32,277 @@
     <t>حالة المشترك</t>
   </si>
   <si>
-    <t>محمد عبدالعزيز عبدالله القحطاني</t>
-  </si>
-  <si>
-    <t>msadeis@outlook.com</t>
-  </si>
-  <si>
-    <t>غير فعال</t>
-  </si>
-  <si>
-    <t>محمد عيسى أحمد عيسى</t>
-  </si>
-  <si>
-    <t>moheis@outlook.com</t>
+    <t>سلمان صلاح سليمان السليمان</t>
+  </si>
+  <si>
+    <t>salman.sss1144@gmail.com</t>
+  </si>
+  <si>
+    <t>فعال</t>
+  </si>
+  <si>
+    <t>العنود ساير السلماني الشمري</t>
+  </si>
+  <si>
+    <t>anood35011@gmail.com</t>
+  </si>
+  <si>
+    <t>اميره سلمان احمد التريكي</t>
+  </si>
+  <si>
+    <t>sweeter.angel_20@gmail.com</t>
+  </si>
+  <si>
+    <t>فاطمه هاشم طاهر السلمان</t>
+  </si>
+  <si>
+    <t>fatimah_hashem1@hotmail.com</t>
+  </si>
+  <si>
+    <t>ملوح عبدالله سعد ال سلمان</t>
+  </si>
+  <si>
+    <t>Malihabdalla@gmail.com</t>
+  </si>
+  <si>
+    <t>علي سلمان ابراهيم العلي</t>
+  </si>
+  <si>
+    <t>Zalali2929@gmil.com</t>
+  </si>
+  <si>
+    <t>اشواق محمد سلمان الغزواني</t>
+  </si>
+  <si>
+    <t>ashwaqalghzwany52@gmail.com</t>
+  </si>
+  <si>
+    <t>عائشه محسن محمد بن سلمان</t>
+  </si>
+  <si>
+    <t>awasha-2013@hotmail.com</t>
+  </si>
+  <si>
+    <t>جنى عصام سلمان الرحيلي</t>
+  </si>
+  <si>
+    <t>ag00agx@gmail.coma</t>
+  </si>
+  <si>
+    <t>أفنان سلمان يحيى الودعاني</t>
+  </si>
+  <si>
+    <t>ageybh99@icloud.com</t>
+  </si>
+  <si>
+    <t>نورة سلمان عبدالله الظفيري</t>
+  </si>
+  <si>
+    <t>nsaldeffeeri@hotmail.com</t>
+  </si>
+  <si>
+    <t>ربى عبدالله محمد ال سلمان</t>
+  </si>
+  <si>
+    <t>rubaabdallah27@gmail.com</t>
+  </si>
+  <si>
+    <t>نوفا سالم سلمان الشمالي</t>
+  </si>
+  <si>
+    <t>maj3ed3ksa@gmail.com</t>
+  </si>
+  <si>
+    <t>هبه عبدالله خليفه السلمان</t>
+  </si>
+  <si>
+    <t>heba-19901@hotmail.com</t>
+  </si>
+  <si>
+    <t>عبدالله سلمان ساير الفريدي</t>
+  </si>
+  <si>
+    <t>assh119@hotmail.com</t>
+  </si>
+  <si>
+    <t>حمود مخلف سلمان الشمري</t>
+  </si>
+  <si>
+    <t>hammod9922@gmail.com</t>
+  </si>
+  <si>
+    <t>سلمان جابر مضواح القحطاني</t>
+  </si>
+  <si>
+    <t>salmain5995@hotmail.com</t>
+  </si>
+  <si>
+    <t>قمر سلمان هادي الفيفي</t>
+  </si>
+  <si>
+    <t>f888a@hotmail.com</t>
+  </si>
+  <si>
+    <t>سلمان عبدالله ناصر الدغيشم</t>
+  </si>
+  <si>
+    <t>adtadta123@icloud.com</t>
+  </si>
+  <si>
+    <t>سلمان عبداله عبدالرحمن السميح</t>
+  </si>
+  <si>
+    <t>ss50000s@hotmail.con</t>
+  </si>
+  <si>
+    <t>زينب سلمان عبدالله الناجم</t>
+  </si>
+  <si>
+    <t>Farohaa2014@gmail.com</t>
+  </si>
+  <si>
+    <t>محمد سلمان رشيد الصقري</t>
+  </si>
+  <si>
+    <t>a7bek1414@hotmail.com</t>
+  </si>
+  <si>
+    <t>ربى سلمان عبدالله الحربي</t>
+  </si>
+  <si>
+    <t>Ruba11ry@gmail.com</t>
+  </si>
+  <si>
+    <t>سلمى سلمان علي البن حاجي</t>
+  </si>
+  <si>
+    <t>Salma210001@hotmail.com</t>
+  </si>
+  <si>
+    <t>انفال احمد سلمان القطيفي</t>
+  </si>
+  <si>
+    <t>anfalahmed1415@gmail.com</t>
+  </si>
+  <si>
+    <t>وفاء عبدالله احمد بن سلمان</t>
+  </si>
+  <si>
+    <t>w.sweet@hotmail.com</t>
+  </si>
+  <si>
+    <t>احمد سلمان عايض الأحمدي</t>
+  </si>
+  <si>
+    <t>ahmed9160a@gmail.com</t>
+  </si>
+  <si>
+    <t>علي سلمان سعيد القحطاني</t>
+  </si>
+  <si>
+    <t>assa-1978@hotmail.com</t>
+  </si>
+  <si>
+    <t>منال بنت سلمان بن صالح النشمي</t>
+  </si>
+  <si>
+    <t>wasm9064@gmail.com</t>
+  </si>
+  <si>
+    <t>محمد راضي سلمان الناصر</t>
+  </si>
+  <si>
+    <t>mhmdalnasr849@gmail.com</t>
+  </si>
+  <si>
+    <t>شيماء سعيد سلمان الردادي</t>
+  </si>
+  <si>
+    <t>sheemalharbi855@gmail.com</t>
+  </si>
+  <si>
+    <t>أمل حنس سلمان العنزي</t>
+  </si>
+  <si>
+    <t>amoolh-123456789@hotmail.com</t>
+  </si>
+  <si>
+    <t>صفاء سلمان جاسم الحرز</t>
+  </si>
+  <si>
+    <t>safa0salman@gmail.com</t>
+  </si>
+  <si>
+    <t>مرام سلمان صالح الحجي</t>
+  </si>
+  <si>
+    <t>mhejji3@gmail.com</t>
+  </si>
+  <si>
+    <t>عبدالرحمن عبدالمنعم سلمان الناجم</t>
+  </si>
+  <si>
+    <t>b65387782@gmail.com</t>
+  </si>
+  <si>
+    <t>سلمان مصلح صالح المالكي</t>
+  </si>
+  <si>
+    <t>slman.m.1440@gmail.com</t>
+  </si>
+  <si>
+    <t>عقل سلمان سعود الشمري</t>
+  </si>
+  <si>
+    <t>aqelshamry@gmail.com</t>
+  </si>
+  <si>
+    <t>أمل سلمان علي المكينه</t>
+  </si>
+  <si>
+    <t>e.amal213@gmail.com</t>
+  </si>
+  <si>
+    <t>عبد العزيز سلمان مرضي المرشد</t>
+  </si>
+  <si>
+    <t>aziz090909az@gmail.com</t>
+  </si>
+  <si>
+    <t>رباب سلمان علي ال جميعان</t>
+  </si>
+  <si>
+    <t>tanoor_12@hotmail.com</t>
+  </si>
+  <si>
+    <t>ايمان سلمان مهدي الشيخ</t>
+  </si>
+  <si>
+    <t>eimanalshaikh@hotmail.com</t>
+  </si>
+  <si>
+    <t>سلمان عياد هليل الشمري</t>
+  </si>
+  <si>
+    <t>sl3sl@hotmail.com</t>
+  </si>
+  <si>
+    <t>بلقيس عبدالله محمد صالح السلمان</t>
+  </si>
+  <si>
+    <t>Balqeesalsalman551@gmail.com</t>
+  </si>
+  <si>
+    <t>خالد سلمان سعد الجعيل</t>
+  </si>
+  <si>
+    <t>juk-123@hotmail.com</t>
+  </si>
+  <si>
+    <t>هاني سلمان محمد الطويل</t>
+  </si>
+  <si>
+    <t>hani1434hani@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -380,7 +638,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" rightToLeft="true">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,6 +688,608 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>